<commit_message>
feat(BulbStateMonitor): add detailed feature requirements and specifications
</commit_message>
<xml_diff>
--- a/BulbStateMonitor/conf.xlsx
+++ b/BulbStateMonitor/conf.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10062\Videos\Desktop\PyUtilDemos\BulbStateMonitor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SanXiaoXing\Desktop\Code\py-util-demos\BulbStateMonitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910F98B3-F736-4E76-A873-8B4BC000EEAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84B535A-C13B-4C8D-B536-98CC26BA7110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-1410" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RS422_State_Light" sheetId="1" r:id="rId1"/>
@@ -31,16 +31,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>INDEX</t>
-  </si>
-  <si>
     <t>SigName</t>
-  </si>
-  <si>
-    <t>ONE</t>
-  </si>
-  <si>
-    <t>ZERO</t>
   </si>
   <si>
     <t>INIT</t>
@@ -1170,6 +1161,18 @@
   </si>
   <si>
     <t>Spare</t>
+  </si>
+  <si>
+    <t>BITE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ActiveState</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>InactiveState</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1555,12 +1558,14 @@
   <dimension ref="A1:F92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="28.21875" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" customWidth="1"/>
     <col min="6" max="6" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1569,19 +1574,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1592,13 +1597,13 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
@@ -1612,13 +1617,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F3" s="2">
         <v>0</v>
@@ -1632,13 +1637,13 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
@@ -1652,13 +1657,13 @@
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F5" s="2">
         <v>0</v>
@@ -1672,13 +1677,13 @@
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F6" s="2">
         <v>0</v>
@@ -1692,13 +1697,13 @@
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
@@ -1712,13 +1717,13 @@
         <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F8" s="2">
         <v>0</v>
@@ -1732,13 +1737,13 @@
         <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F9" s="2">
         <v>0</v>
@@ -1752,13 +1757,13 @@
         <v>0</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F10" s="2">
         <v>0</v>
@@ -1772,13 +1777,13 @@
         <v>1</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F11" s="2">
         <v>0</v>
@@ -1792,13 +1797,13 @@
         <v>2</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F12" s="2">
         <v>0</v>
@@ -1812,13 +1817,13 @@
         <v>3</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F13" s="2">
         <v>0</v>
@@ -1832,13 +1837,13 @@
         <v>4</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F14" s="2">
         <v>0</v>
@@ -1852,13 +1857,13 @@
         <v>5</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F15" s="2">
         <v>0</v>
@@ -1872,13 +1877,13 @@
         <v>6</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F16" s="2">
         <v>0</v>
@@ -1892,13 +1897,13 @@
         <v>7</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F17" s="2">
         <v>0</v>
@@ -1912,13 +1917,13 @@
         <v>0</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F18" s="2">
         <v>0</v>
@@ -1932,13 +1937,13 @@
         <v>1</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F19" s="2">
         <v>0</v>
@@ -1952,13 +1957,13 @@
         <v>2</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F20" s="2">
         <v>0</v>
@@ -1972,13 +1977,13 @@
         <v>3</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F21" s="2">
         <v>0</v>
@@ -1992,13 +1997,13 @@
         <v>4</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F22" s="2">
         <v>0</v>
@@ -2012,13 +2017,13 @@
         <v>5</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F23" s="2">
         <v>0</v>
@@ -2032,13 +2037,13 @@
         <v>6</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F24" s="2">
         <v>0</v>
@@ -2052,13 +2057,13 @@
         <v>7</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F25" s="2">
         <v>0</v>
@@ -2072,13 +2077,13 @@
         <v>0</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F26" s="2">
         <v>0</v>
@@ -2092,13 +2097,13 @@
         <v>1</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F27" s="2">
         <v>0</v>
@@ -2112,13 +2117,13 @@
         <v>2</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F28" s="2">
         <v>0</v>
@@ -2132,13 +2137,13 @@
         <v>3</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F29" s="2">
         <v>0</v>
@@ -2152,13 +2157,13 @@
         <v>4</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F30" s="2">
         <v>0</v>
@@ -2172,13 +2177,13 @@
         <v>5</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F31" s="2">
         <v>0</v>
@@ -2192,13 +2197,13 @@
         <v>6</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F32" s="2">
         <v>0</v>
@@ -2212,13 +2217,13 @@
         <v>7</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F33" s="2">
         <v>0</v>
@@ -2232,13 +2237,13 @@
         <v>0</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F34" s="2">
         <v>0</v>
@@ -2252,13 +2257,13 @@
         <v>1</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F35" s="2">
         <v>0</v>
@@ -2272,13 +2277,13 @@
         <v>2</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F36" s="2">
         <v>0</v>
@@ -2292,13 +2297,13 @@
         <v>3</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F37" s="2">
         <v>0</v>
@@ -2312,13 +2317,13 @@
         <v>4</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F38" s="2">
         <v>0</v>
@@ -2332,13 +2337,13 @@
         <v>5</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F39" s="2">
         <v>0</v>
@@ -2352,13 +2357,13 @@
         <v>6</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F40" s="2">
         <v>0</v>
@@ -2372,13 +2377,13 @@
         <v>7</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F41" s="2">
         <v>0</v>
@@ -2392,13 +2397,13 @@
         <v>0</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F42" s="2">
         <v>0</v>
@@ -2412,13 +2417,13 @@
         <v>1</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F43" s="2">
         <v>0</v>
@@ -2432,13 +2437,13 @@
         <v>2</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F44" s="2">
         <v>0</v>
@@ -2452,13 +2457,13 @@
         <v>3</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F45" s="2">
         <v>0</v>
@@ -2472,13 +2477,13 @@
         <v>4</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F46" s="2">
         <v>0</v>
@@ -2492,13 +2497,13 @@
         <v>5</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F47" s="2">
         <v>0</v>
@@ -2512,13 +2517,13 @@
         <v>6</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F48" s="2">
         <v>0</v>
@@ -2532,13 +2537,13 @@
         <v>7</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F49" s="2">
         <v>0</v>
@@ -2552,13 +2557,13 @@
         <v>0</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F50" s="2">
         <v>0</v>
@@ -2572,13 +2577,13 @@
         <v>1</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F51" s="2">
         <v>0</v>
@@ -2592,13 +2597,13 @@
         <v>2</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F52" s="2">
         <v>0</v>
@@ -2612,13 +2617,13 @@
         <v>3</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F53" s="2">
         <v>0</v>
@@ -2632,13 +2637,13 @@
         <v>4</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F54" s="2">
         <v>0</v>
@@ -2652,13 +2657,13 @@
         <v>5</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F55" s="2">
         <v>0</v>
@@ -2672,13 +2677,13 @@
         <v>6</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F56" s="2">
         <v>0</v>
@@ -2692,13 +2697,13 @@
         <v>7</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F57" s="2">
         <v>0</v>
@@ -2712,13 +2717,13 @@
         <v>0</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F58" s="2">
         <v>0</v>
@@ -2732,13 +2737,13 @@
         <v>1</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F59" s="2">
         <v>0</v>
@@ -2752,13 +2757,13 @@
         <v>2</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F60" s="2">
         <v>0</v>
@@ -2772,13 +2777,13 @@
         <v>3</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F61" s="2">
         <v>0</v>
@@ -2792,13 +2797,13 @@
         <v>4</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F62" s="2">
         <v>0</v>
@@ -2812,13 +2817,13 @@
         <v>7</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F63" s="2">
         <v>0</v>
@@ -2832,13 +2837,13 @@
         <v>0</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F64" s="2">
         <v>0</v>
@@ -2852,13 +2857,13 @@
         <v>1</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F65" s="2">
         <v>0</v>
@@ -2872,13 +2877,13 @@
         <v>2</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F66" s="2">
         <v>0</v>
@@ -2892,13 +2897,13 @@
         <v>3</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F67" s="2">
         <v>0</v>
@@ -2912,13 +2917,13 @@
         <v>4</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F68" s="2">
         <v>0</v>
@@ -2932,13 +2937,13 @@
         <v>5</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F69" s="2">
         <v>0</v>
@@ -2952,13 +2957,13 @@
         <v>6</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F70" s="2">
         <v>0</v>
@@ -2972,13 +2977,13 @@
         <v>7</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F71" s="2">
         <v>0</v>
@@ -2992,13 +2997,13 @@
         <v>0</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F72" s="2">
         <v>0</v>
@@ -3012,13 +3017,13 @@
         <v>1</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F73" s="2">
         <v>0</v>
@@ -3032,13 +3037,13 @@
         <v>2</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F74" s="2">
         <v>0</v>
@@ -3052,13 +3057,13 @@
         <v>3</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F75" s="2">
         <v>0</v>
@@ -3072,13 +3077,13 @@
         <v>4</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F76" s="2">
         <v>0</v>
@@ -3092,13 +3097,13 @@
         <v>5</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F77" s="2">
         <v>0</v>
@@ -3112,13 +3117,13 @@
         <v>6</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F78" s="2">
         <v>0</v>
@@ -3132,13 +3137,13 @@
         <v>7</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F79" s="2">
         <v>0</v>
@@ -3152,13 +3157,13 @@
         <v>0</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F80" s="2">
         <v>0</v>
@@ -3172,13 +3177,13 @@
         <v>1</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F81" s="2">
         <v>0</v>
@@ -3192,13 +3197,13 @@
         <v>5</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F82" s="2">
         <v>0</v>
@@ -3212,13 +3217,13 @@
         <v>6</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F83" s="2">
         <v>0</v>
@@ -3232,13 +3237,13 @@
         <v>7</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F84" s="2">
         <v>0</v>
@@ -3252,13 +3257,13 @@
         <v>0</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F85" s="2">
         <v>0</v>
@@ -3272,13 +3277,13 @@
         <v>1</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F86" s="2">
         <v>0</v>
@@ -3292,13 +3297,13 @@
         <v>2</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F87" s="2">
         <v>0</v>
@@ -3312,13 +3317,13 @@
         <v>3</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F88" s="2">
         <v>0</v>
@@ -3332,13 +3337,13 @@
         <v>4</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F89" s="2">
         <v>0</v>
@@ -3352,13 +3357,13 @@
         <v>5</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F90" s="2">
         <v>0</v>
@@ -3372,13 +3377,13 @@
         <v>6</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F91" s="2">
         <v>0</v>
@@ -3392,13 +3397,13 @@
         <v>7</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F92" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
feat(BulbStateMonitor): add data input functionality and improve performance
</commit_message>
<xml_diff>
--- a/BulbStateMonitor/conf.xlsx
+++ b/BulbStateMonitor/conf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SanXiaoXing\Desktop\Code\py-util-demos\BulbStateMonitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A486DF-A66A-4A53-AEFA-85EC3C589714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD2BFD1-64FA-48FC-9003-E989E5EA0159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1224" yWindow="1764" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RS422_State_Light" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="96">
   <si>
     <t>BYTE</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1173,6 +1173,10 @@
   </si>
   <si>
     <t>SignalName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>故障</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1558,8 +1562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D6" activeCellId="1" sqref="E6 D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1604,7 +1608,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>4</v>
+        <v>95</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
@@ -1624,7 +1628,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>4</v>
+        <v>95</v>
       </c>
       <c r="F3" s="2">
         <v>0</v>
@@ -1644,7 +1648,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>4</v>
+        <v>95</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
@@ -1664,7 +1668,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>4</v>
+        <v>95</v>
       </c>
       <c r="F5" s="2">
         <v>0</v>

</xml_diff>